<commit_message>
Version finale du cahier des charges
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_previsionnel_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_previsionnel_travail_de_diplome.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\bj-travail-diplome-2021\documentation\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JO-PC\Desktop\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA0E42D-80B9-4279-817D-847DB9EC9B16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -165,15 +166,9 @@
     <t>Onglet calendrier</t>
   </si>
   <si>
-    <t>Onglet contenue séances</t>
-  </si>
-  <si>
     <t>Éducateur canin</t>
   </si>
   <si>
-    <t>Onglet d'affichage de tout les clients</t>
-  </si>
-  <si>
     <t>Onglet de création de fiche client préliminaire</t>
   </si>
   <si>
@@ -181,12 +176,6 @@
   </si>
   <si>
     <t>Onglet de valdiation de fiche client</t>
-  </si>
-  <si>
-    <t>Onglet des contenues séances d'un client</t>
-  </si>
-  <si>
-    <t>Onglet d'ajout de document</t>
   </si>
   <si>
     <t>Fonctionnalités</t>
@@ -263,16 +252,28 @@
     <t>Connexion</t>
   </si>
   <si>
-    <t>Gestion des dissponiblités de l'éducateur canin</t>
-  </si>
-  <si>
     <t>Progressive web app</t>
+  </si>
+  <si>
+    <t>Onglet contenu séances</t>
+  </si>
+  <si>
+    <t>Onglet d'affichage de tous les clients</t>
+  </si>
+  <si>
+    <t>Onglet des contenus séances d'un client</t>
+  </si>
+  <si>
+    <t>Onglet d'ajout de documents</t>
+  </si>
+  <si>
+    <t>Gestion des disponiblités de l'éducateur canin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.m"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -787,6 +788,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,9 +810,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1099,7 +1100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1107,7 +1108,7 @@
   <dimension ref="A1:BT39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="V2" s="24" t="s">
         <v>35</v>
@@ -1338,7 +1339,7 @@
         <v>27</v>
       </c>
       <c r="AB2" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AC2" s="23" t="s">
         <v>28</v>
@@ -1383,10 +1384,10 @@
         <v>43</v>
       </c>
       <c r="AQ2" s="50" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AR2" s="66" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AS2" s="17">
         <v>8</v>
@@ -1400,7 +1401,7 @@
     </row>
     <row r="3" spans="1:72" s="16" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="37"/>
@@ -1456,7 +1457,7 @@
     </row>
     <row r="4" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="64"/>
@@ -1500,10 +1501,10 @@
       <c r="AO4" s="59"/>
       <c r="AP4" s="63"/>
       <c r="AQ4" s="41"/>
-      <c r="AR4" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS4" s="67">
+      <c r="AR4" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS4" s="68">
         <v>3.125E-2</v>
       </c>
       <c r="AT4" s="2"/>
@@ -1584,11 +1585,11 @@
       <c r="AO5" s="58"/>
       <c r="AP5" s="60"/>
       <c r="AQ5" s="20">
-        <f>SUM(C5:AP5)</f>
-        <v>4</v>
-      </c>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="68"/>
+        <f t="shared" ref="AQ5:AQ10" si="0">SUM(C5:AP5)</f>
+        <v>4</v>
+      </c>
+      <c r="AR5" s="73"/>
+      <c r="AS5" s="69"/>
     </row>
     <row r="6" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1642,13 +1643,13 @@
       <c r="AO6" s="58"/>
       <c r="AP6" s="60"/>
       <c r="AQ6" s="20">
-        <f>SUM(C6:AP6)</f>
-        <v>4</v>
-      </c>
-      <c r="AR6" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS6" s="69">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AR6" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS6" s="70">
         <v>300</v>
       </c>
     </row>
@@ -1706,15 +1707,15 @@
       <c r="AO7" s="58"/>
       <c r="AP7" s="60"/>
       <c r="AQ7" s="20">
-        <f>SUM(C7:AP7)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AR7" s="72"/>
-      <c r="AS7" s="70"/>
+      <c r="AR7" s="73"/>
+      <c r="AS7" s="71"/>
     </row>
     <row r="8" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" s="18">
         <v>8</v>
@@ -1764,15 +1765,15 @@
       <c r="AO8" s="58"/>
       <c r="AP8" s="60"/>
       <c r="AQ8" s="20">
-        <f>SUM(C8:AP8)</f>
-        <v>8</v>
-      </c>
-      <c r="AR8" s="74"/>
-      <c r="AS8" s="74"/>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AR8" s="67"/>
+      <c r="AS8" s="67"/>
     </row>
     <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9" s="18">
         <v>16</v>
@@ -1826,15 +1827,15 @@
       <c r="AO9" s="58"/>
       <c r="AP9" s="60"/>
       <c r="AQ9" s="20">
-        <f>SUM(C9:AP9)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AR9" s="74"/>
-      <c r="AS9" s="74"/>
+      <c r="AR9" s="67"/>
+      <c r="AS9" s="67"/>
     </row>
     <row r="10" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B10" s="18">
         <v>4</v>
@@ -1882,11 +1883,11 @@
       <c r="AO10" s="58"/>
       <c r="AP10" s="60"/>
       <c r="AQ10" s="20">
-        <f>SUM(C10:AP10)</f>
-        <v>4</v>
-      </c>
-      <c r="AR10" s="74"/>
-      <c r="AS10" s="74"/>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AR10" s="67"/>
+      <c r="AS10" s="67"/>
     </row>
     <row r="11" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
@@ -2042,7 +2043,7 @@
     </row>
     <row r="13" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B13" s="20">
         <v>4</v>
@@ -2214,7 +2215,7 @@
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B16" s="20">
         <v>8</v>
@@ -2272,7 +2273,7 @@
     </row>
     <row r="17" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="64"/>
@@ -2348,7 +2349,7 @@
     </row>
     <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B18" s="20">
         <v>4</v>
@@ -2462,7 +2463,7 @@
     </row>
     <row r="20" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="20">
         <v>4</v>
@@ -2518,7 +2519,7 @@
     </row>
     <row r="21" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="20">
         <v>4</v>
@@ -2574,7 +2575,7 @@
     </row>
     <row r="22" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" s="20">
         <v>4</v>
@@ -2632,7 +2633,7 @@
     </row>
     <row r="23" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B23" s="20">
         <v>4</v>
@@ -2680,7 +2681,7 @@
       <c r="AO23" s="58"/>
       <c r="AP23" s="60"/>
       <c r="AQ23" s="20">
-        <f t="shared" ref="AQ18:AQ24" si="0">SUM(C23:AP23)</f>
+        <f t="shared" ref="AQ23" si="1">SUM(C23:AP23)</f>
         <v>4</v>
       </c>
       <c r="AR23" s="49"/>
@@ -2688,7 +2689,7 @@
     </row>
     <row r="24" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B24" s="20">
         <v>4</v>
@@ -2744,7 +2745,7 @@
     </row>
     <row r="25" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="64"/>
@@ -2820,7 +2821,7 @@
     </row>
     <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B26" s="20">
         <v>8</v>
@@ -2870,7 +2871,7 @@
       <c r="AO26" s="58"/>
       <c r="AP26" s="60"/>
       <c r="AQ26" s="20">
-        <f>SUM(C26:AP26)</f>
+        <f t="shared" ref="AQ26:AQ35" si="2">SUM(C26:AP26)</f>
         <v>8</v>
       </c>
       <c r="AR26" s="49"/>
@@ -2878,7 +2879,7 @@
     </row>
     <row r="27" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" s="20">
         <v>6</v>
@@ -2926,7 +2927,7 @@
       <c r="AO27" s="58"/>
       <c r="AP27" s="60"/>
       <c r="AQ27" s="20">
-        <f>SUM(C27:AP27)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AR27" s="49"/>
@@ -2934,7 +2935,7 @@
     </row>
     <row r="28" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B28" s="20">
         <v>6</v>
@@ -2982,7 +2983,7 @@
       <c r="AO28" s="58"/>
       <c r="AP28" s="60"/>
       <c r="AQ28" s="20">
-        <f>SUM(C28:AP28)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AR28" s="49"/>
@@ -2990,7 +2991,7 @@
     </row>
     <row r="29" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" s="20">
         <v>8</v>
@@ -3040,7 +3041,7 @@
       <c r="AO29" s="58"/>
       <c r="AP29" s="60"/>
       <c r="AQ29" s="20">
-        <f>SUM(C29:AP29)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AR29" s="49"/>
@@ -3048,7 +3049,7 @@
     </row>
     <row r="30" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B30" s="20">
         <v>16</v>
@@ -3100,7 +3101,7 @@
       <c r="AO30" s="58"/>
       <c r="AP30" s="60"/>
       <c r="AQ30" s="20">
-        <f>SUM(C30:AP30)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="AR30" s="49"/>
@@ -3108,7 +3109,7 @@
     </row>
     <row r="31" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B31" s="20">
         <v>8</v>
@@ -3158,7 +3159,7 @@
       <c r="AO31" s="58"/>
       <c r="AP31" s="60"/>
       <c r="AQ31" s="20">
-        <f>SUM(C31:AP31)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AR31" s="49"/>
@@ -3166,7 +3167,7 @@
     </row>
     <row r="32" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B32" s="20">
         <v>8</v>
@@ -3216,7 +3217,7 @@
       <c r="AO32" s="58"/>
       <c r="AP32" s="60"/>
       <c r="AQ32" s="20">
-        <f>SUM(C32:AP32)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AR32" s="49"/>
@@ -3224,7 +3225,7 @@
     </row>
     <row r="33" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" s="20">
         <v>8</v>
@@ -3274,7 +3275,7 @@
       <c r="AO33" s="58"/>
       <c r="AP33" s="60"/>
       <c r="AQ33" s="20">
-        <f>SUM(C33:AP33)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AR33" s="49"/>
@@ -3282,7 +3283,7 @@
     </row>
     <row r="34" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B34" s="20">
         <v>16</v>
@@ -3334,7 +3335,7 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="60"/>
       <c r="AQ34" s="20">
-        <f>SUM(C34:AP34)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="AR34" s="49"/>
@@ -3342,7 +3343,7 @@
     </row>
     <row r="35" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B35" s="20">
         <v>10</v>
@@ -3394,7 +3395,7 @@
       <c r="AO35" s="58"/>
       <c r="AP35" s="60"/>
       <c r="AQ35" s="20">
-        <f>SUM(C35:AP35)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AR35" s="49"/>
@@ -3478,7 +3479,7 @@
     </row>
     <row r="37" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" s="20">
         <v>68</v>
@@ -3608,7 +3609,7 @@
     </row>
     <row r="38" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B38" s="21">
         <v>38</v>
@@ -3738,171 +3739,171 @@
     </row>
     <row r="39" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="22">
-        <f>SUM(B4:B38)</f>
+        <f t="shared" ref="B39:AQ39" si="3">SUM(B4:B38)</f>
         <v>300</v>
       </c>
       <c r="C39">
-        <f>SUM(C4:C38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D39" s="22">
-        <f>SUM(D4:D38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E39">
-        <f>SUM(E4:E38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F39" s="22">
-        <f>SUM(F4:F38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G39">
-        <f>SUM(G4:G38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H39" s="22">
-        <f>SUM(H4:H38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I39" s="22">
-        <f>SUM(I4:I38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="J39">
-        <f>SUM(J4:J38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="K39" s="22">
-        <f>SUM(K4:K38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L39">
-        <f>SUM(L4:L38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="M39" s="22">
-        <f>SUM(M4:M38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N39">
-        <f>SUM(N4:N38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O39" s="22">
-        <f>SUM(O4:O38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="P39" s="22">
-        <f>SUM(P4:P38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Q39">
-        <f>SUM(Q4:Q38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="R39" s="22">
-        <f>SUM(R4:R38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="S39">
-        <f>SUM(S4:S38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="T39" s="22">
-        <f>SUM(T4:T38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U39">
-        <f>SUM(U4:U38)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V39" s="22">
-        <f>SUM(V4:V38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W39" s="22">
-        <f>SUM(W4:W38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="X39">
-        <f>SUM(X4:X38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Y39" s="22">
-        <f>SUM(Y4:Y38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Z39">
-        <f>SUM(Z4:Z38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AA39" s="22">
-        <f>SUM(AA4:AA38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AB39">
-        <f>SUM(AB4:AB38)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC39" s="22">
-        <f>SUM(AC4:AC38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AD39" s="22">
-        <f>SUM(AD4:AD38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AE39">
-        <f>SUM(AE4:AE38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AF39" s="22">
-        <f>SUM(AF4:AF38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AG39">
-        <f>SUM(AG4:AG38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AH39" s="22">
-        <f>SUM(AH4:AH38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AI39">
-        <f>SUM(AI4:AI38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AJ39" s="22">
-        <f>SUM(AJ4:AJ38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AK39" s="22">
-        <f>SUM(AK4:AK38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AL39">
-        <f>SUM(AL4:AL38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AM39" s="22">
-        <f>SUM(AM4:AM38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AN39">
-        <f>SUM(AN4:AN38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AO39" s="22">
-        <f>SUM(AO4:AO38)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AP39">
-        <f>SUM(AP4:AP38)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="AQ39" s="22">
-        <f>SUM(AQ4:AQ38)</f>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="AR39" s="49"/>

</xml_diff>